<commit_message>
[Thực hành] Hợp nhất các cột dữ liệu từ nhiều data frame
</commit_message>
<xml_diff>
--- a/2. Python for DA/Link record.xlsx
+++ b/2. Python for DA/Link record.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hung\Desktop\Học\Codegym\Codegym\2. Python for DA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1724889F-7D68-474C-A01A-D54CE12C37BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF3C42BF-9EBC-4060-8901-50B1CCE428BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="39">
   <si>
     <t>Ngày</t>
   </si>
@@ -120,6 +120,39 @@
   </si>
   <si>
     <t>Done</t>
+  </si>
+  <si>
+    <t>https://zoom.us/rec/play/9rqDVSztxqxx7-GqyKcIREg9doHHfcbPMxhmBDXxY4nMt5OQcfjDJnOJXl1vyycvXAmuWPTpYCMumy3H.S780cc3gEc40E39v?continueMode=true&amp;_x_zm_rtaid=wwSi-ScIRa2lw1QLNM3sOw.1669538040676.1ddd9f75194d27c04e9ba5973bde60bd&amp;_x_zm_rhtaid=55</t>
+  </si>
+  <si>
+    <t>https://zoom.us/rec/play/N6NVnKqOwe9i8DoJ4rm-yA5aylNS4qMFdWws485gQZwyVTG-KpSJ6AriGcMJ1tQCNDETmXHyHZi_zEZd.tMBaisORe59gaxdj?continueMode=true&amp;_x_zm_rtaid=wwSi-ScIRa2lw1QLNM3sOw.1669538040676.1ddd9f75194d27c04e9ba5973bde60bd&amp;_x_zm_rhtaid=55</t>
+  </si>
+  <si>
+    <t>https://zoom.us/rec/play/3sSzhbXVUxDmrZiee-D-EjM01Wq3M0dWx59K8FrDZoqkv_zQq8YJtI0Y0biHe902suF-m4WfjEe_EyxJ.12UAZfkyH5YeQJXh?continueMode=true&amp;_x_zm_rtaid=wwSi-ScIRa2lw1QLNM3sOw.1669538040676.1ddd9f75194d27c04e9ba5973bde60bd&amp;_x_zm_rhtaid=55</t>
+  </si>
+  <si>
+    <t>https://zoom.us/rec/share/2LjjCHY9RWe7FCyZwYw6RV33UcA2isYTxViuTZSmRSE_Xz01v6fmd9IXGTmaArFP.A-nETf4bqQJaTzY4</t>
+  </si>
+  <si>
+    <t>https://zoom.us/rec/share/-EIvE6woZ6rGdxM3kp8S--yjsipOuKCXmq0l8JIhdmSLwU2JqspYCSUhIWrYWHzi.On8k-WEOislNXqse</t>
+  </si>
+  <si>
+    <t>https://zoom.us/rec/play/l4g6LCEmLrR_3rqSp8zcxzhVHjas0Skxm-r8CUIIMs40HqfESw6oZqpsQkrKXXquJ19IEYvSSfgYdfCM.Lo2BMtRTYRKM_sjb?continueMode=true&amp;_x_zm_rtaid=LS47qZHbS0Csx8jjRCN8dw.1670731521042.b3d473194791c9e526111e4bb6fde81d&amp;_x_zm_rhtaid=184</t>
+  </si>
+  <si>
+    <t>https://zoom.us/rec/play/kq4kxIHxTiLImTAXQTO2tXjvRDdFJdbyZgwIpQfKZFGaR7z-tS3kyDzX74OJwC9GHOZGBhgL3qfr5CWI.3tzz4IHhXSlRV5KR?continueMode=true&amp;_x_zm_rtaid=LS47qZHbS0Csx8jjRCN8dw.1670731521042.b3d473194791c9e526111e4bb6fde81d&amp;_x_zm_rhtaid=184</t>
+  </si>
+  <si>
+    <t>https://zoom.us/rec/play/La9gRWETlob4q0PaROzEXHYBVFHR-PBqzwn8V53yYjN9vELZj-BRw2c6mb5EAPuoqp1MglBlwB9I3MPh.uJYcvUXWI2REjjL2?continueMode=true&amp;_x_zm_rtaid=LS47qZHbS0Csx8jjRCN8dw.1670731521042.b3d473194791c9e526111e4bb6fde81d&amp;_x_zm_rhtaid=184</t>
+  </si>
+  <si>
+    <t>https://zoom.us/rec/play/qyDcgMrywA0CHSDPN5NMnXLSCWBuwFcTFl9H2gLdhN11rFC0tV3zzUOgJYivBSyMihR-M7J4ZRCtAGGM.dawIYKXdhkPzQ_L6?continueMode=true&amp;_x_zm_rtaid=LS47qZHbS0Csx8jjRCN8dw.1670731521042.b3d473194791c9e526111e4bb6fde81d&amp;_x_zm_rhtaid=184</t>
+  </si>
+  <si>
+    <t>https://zoom.us/rec/play/CWxosEUV0uL2gVVPINeyzTKj-9eum8WwU0f9ZSFEiIvxNcNEDaC_OHbrVkZZrH-XTwOWOAgoWAvAGW9s.J7agLk-oR748wYhX?continueMode=true&amp;_x_zm_rtaid=LS47qZHbS0Csx8jjRCN8dw.1670731521042.b3d473194791c9e526111e4bb6fde81d&amp;_x_zm_rhtaid=184</t>
+  </si>
+  <si>
+    <t>https://zoom.us/rec/play/1nf8LBaxQW3edx05w0EET8hdNkyhn4Y2o-ZxsQlDSNxbV1BnmXscVmY5lT_rxpTcdeuvGR3i4dAggYXV.tzWuwy7yvm3Qi-P5?continueMode=true&amp;_x_zm_rtaid=LS47qZHbS0Csx8jjRCN8dw.1670731521042.b3d473194791c9e526111e4bb6fde81d&amp;_x_zm_rhtaid=184</t>
   </si>
 </sst>
 </file>
@@ -449,17 +482,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="D3:H23"/>
+  <dimension ref="D3:H34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="3" width="9.140625" style="2"/>
     <col min="4" max="4" width="18.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="117.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="117.5703125" style="3" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="19.140625" style="2" bestFit="1" customWidth="1"/>
     <col min="7" max="16384" width="9.140625" style="2"/>
   </cols>
@@ -468,7 +501,7 @@
       <c r="D3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="3" t="s">
         <v>1</v>
       </c>
       <c r="F3" s="2" t="s">
@@ -479,7 +512,6 @@
       <c r="D4" s="1">
         <v>44834</v>
       </c>
-      <c r="E4" s="3"/>
       <c r="F4" s="3" t="s">
         <v>3</v>
       </c>
@@ -718,6 +750,94 @@
       <c r="F23" s="3"/>
       <c r="G23" s="3"/>
       <c r="H23" s="3"/>
+    </row>
+    <row r="24" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D24" s="1">
+        <v>44881</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="25" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D25" s="1">
+        <v>44883</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="26" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D26" s="1">
+        <v>44886</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="27" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D27" s="1">
+        <v>44888</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="28" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D28" s="1">
+        <v>44890</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="29" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D29" s="1">
+        <v>44893</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="30" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D30" s="1">
+        <v>44895</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="31" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D31" s="1">
+        <v>44897</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="32" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D32" s="1">
+        <v>44900</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="33" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D33" s="1">
+        <v>44902</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="34" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D34" s="1">
+        <v>44904</v>
+      </c>
+      <c r="E34" s="3" t="s">
+        <v>38</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Prepare for case study
</commit_message>
<xml_diff>
--- a/2. Python for DA/Link record.xlsx
+++ b/2. Python for DA/Link record.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hung\Desktop\Học\Codegym\Codegym\2. Python for DA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF3C42BF-9EBC-4060-8901-50B1CCE428BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4800BD56-352D-415E-A98F-F4DE1B3CFCEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="48">
   <si>
     <t>Ngày</t>
   </si>
@@ -153,6 +153,33 @@
   </si>
   <si>
     <t>https://zoom.us/rec/play/1nf8LBaxQW3edx05w0EET8hdNkyhn4Y2o-ZxsQlDSNxbV1BnmXscVmY5lT_rxpTcdeuvGR3i4dAggYXV.tzWuwy7yvm3Qi-P5?continueMode=true&amp;_x_zm_rtaid=LS47qZHbS0Csx8jjRCN8dw.1670731521042.b3d473194791c9e526111e4bb6fde81d&amp;_x_zm_rhtaid=184</t>
+  </si>
+  <si>
+    <t>https://zoom.us/rec/share/U-GB6_oep1BC7i1Pi_YZW96fh6u3ZtCm2vqYghfLkHT7T4X1tg6mkJKH6C0sJ4yx.BooSWKSJUtkO_FnK</t>
+  </si>
+  <si>
+    <t>https://zoom.us/rec/share/Psrs6H-mVO7Vf_tbnlVJbsffZs5vuL1phykJSYkR35uZvLvqOJdOA2Ydf3dcXY4p.OtLAMDM3tEY5jE13</t>
+  </si>
+  <si>
+    <t>https://zoom.us/rec/share/9k79XAVdCgQEtyN-gHK0aElB-eS9wxbHniJpqUtaiDiZKd2p2HE1LYETsjlJuHm9.2zELiyX7ZuG1BiMR</t>
+  </si>
+  <si>
+    <t>https://zoom.us/rec/share/40jbucMo5iPRva_a2X6fNEnz-z5D2yWjsyXMdfrjgbXW2Mft8Va1dV9aszQAQ-BV.Z2g9Ywbj-zSgC52D</t>
+  </si>
+  <si>
+    <t>https://zoom.us/rec/share/S6_IqmA2fQA8vb-AF8c3X3nwAgEZUL_yCWWTsyI_blAqMhYU9tyxnIazMBUv7u6N.mMh9RREU9nxf4Jk4</t>
+  </si>
+  <si>
+    <t>https://zoom.us/rec/share/-Ryk4BEGQNEkjKkeGA3q_8HUT-XE8F76UdGU1y2N0luxB4XKmBQa60oi0Rql4Nr1.bIwqmW_DQLI6fW9A</t>
+  </si>
+  <si>
+    <t>Nghỉ??</t>
+  </si>
+  <si>
+    <t>https://zoom.us/rec/share/x8QSnXuJoJn5OEtSVVtK6hdWcyMeuckQSMNTAzCwkXApN7yBkzk0jGZNk9lW2USJ.p2n9T7RCiC6eQRSQ</t>
+  </si>
+  <si>
+    <t>https://zoom.us/rec/share/CQ35g_0cFAOENXmBJcM_XwMdhWc_XDbxxTMuIoe-UlhD4_WjhDV0jgN4N66Kz39W.Rz0rmKwKEp5BonWA</t>
   </si>
 </sst>
 </file>
@@ -482,10 +509,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="D3:H34"/>
+  <dimension ref="D3:H46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E34" sqref="E34"/>
+      <pane xSplit="3" ySplit="3" topLeftCell="D16" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="D1" sqref="D1"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
+      <selection pane="bottomRight" activeCell="E42" sqref="E42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -608,7 +638,9 @@
       <c r="F11" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G11" s="3"/>
+      <c r="G11" s="3" t="s">
+        <v>27</v>
+      </c>
       <c r="H11" s="3"/>
     </row>
     <row r="12" spans="4:8" x14ac:dyDescent="0.25">
@@ -621,7 +653,9 @@
       <c r="F12" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="G12" s="3"/>
+      <c r="G12" s="3" t="s">
+        <v>27</v>
+      </c>
       <c r="H12" s="3"/>
     </row>
     <row r="13" spans="4:8" x14ac:dyDescent="0.25">
@@ -634,7 +668,9 @@
       <c r="F13" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="G13" s="3"/>
+      <c r="G13" s="3" t="s">
+        <v>27</v>
+      </c>
       <c r="H13" s="3"/>
     </row>
     <row r="14" spans="4:8" x14ac:dyDescent="0.25">
@@ -837,6 +873,99 @@
       </c>
       <c r="E34" s="3" t="s">
         <v>38</v>
+      </c>
+    </row>
+    <row r="35" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D35" s="1">
+        <v>44907</v>
+      </c>
+      <c r="E35" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="36" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D36" s="1">
+        <v>44909</v>
+      </c>
+      <c r="E36" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="37" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D37" s="1">
+        <v>44911</v>
+      </c>
+      <c r="E37" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="38" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D38" s="1">
+        <v>44914</v>
+      </c>
+      <c r="E38" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="39" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D39" s="1">
+        <v>44916</v>
+      </c>
+      <c r="E39" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="40" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D40" s="1">
+        <v>44918</v>
+      </c>
+      <c r="E40" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="41" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D41" s="1">
+        <v>44921</v>
+      </c>
+      <c r="E41" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="42" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D42" s="1">
+        <v>44923</v>
+      </c>
+      <c r="E42" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="43" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D43" s="1">
+        <v>44925</v>
+      </c>
+      <c r="E43" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="44" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D44" s="1">
+        <v>44928</v>
+      </c>
+      <c r="E44" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="45" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D45" s="1">
+        <v>44930</v>
+      </c>
+      <c r="E45" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="46" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D46" s="1">
+        <v>44932</v>
       </c>
     </row>
   </sheetData>

</xml_diff>